<commit_message>
Remove hydrologic scenarios line. Add 9-year plot Powell 10-year
</commit_message>
<xml_diff>
--- a/Powell10year/Curtailment.xlsx
+++ b/Powell10year/Curtailment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20374"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20378"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverFutures\Powell10year\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCoding2\Powell10year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C60FA16-2DE4-4AB3-AA43-B3D5C8721646}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1615AEDF-F96A-4A0F-AFE8-B9604535AE47}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6640" xr2:uid="{BB94B92A-C8EF-4BFC-A8C8-F3C66B3235F7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6640" activeTab="3" xr2:uid="{BB94B92A-C8EF-4BFC-A8C8-F3C66B3235F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Curtailment" sheetId="1" r:id="rId1"/>
@@ -2212,6 +2212,56 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.10753280381544726"/>
+                  <c:y val="0.33244469342134914"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'UpperBasin Consumptive Use'!$E$2:$E$59</c:f>
@@ -4646,7 +4696,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{D2AB4D09-0447-48BE-916C-B60B79506CA2}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="76" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="78" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4657,7 +4707,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{F5B431A8-98CE-47C3-9056-B2E83CB04BE9}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="76" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="78" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4668,7 +4718,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{292F6C87-5A69-437D-9485-8743CC210C56}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="76" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="78" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4679,7 +4729,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="12996612" cy="9437270"/>
+    <xdr:ext cx="12993077" cy="9439519"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -4712,7 +4762,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="12996612" cy="9437270"/>
+    <xdr:ext cx="12993077" cy="9439519"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -4745,7 +4795,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="12954000" cy="9429750"/>
+    <xdr:ext cx="12993077" cy="9439519"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -5073,7 +5123,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96D20514-3706-4FB6-85B8-266E69D78861}">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:F9"/>
     </sheetView>
   </sheetViews>
@@ -5594,7 +5644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{029FAB00-0168-4CAE-B73F-AB81DA5737F2}">
   <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>

</xml_diff>